<commit_message>
Cration des mêmes pages que dans le projet WPF Page de desinscription , bouton menu aléatoire pouvoir sélectionné plusieurs article dans la liste de course pour supprimé
</commit_message>
<xml_diff>
--- a/Idée amélioration appli.xlsx
+++ b/Idée amélioration appli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francois\source\repos\LoGeCui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD8B89B-EEBB-42B3-B054-74CD5C4BD1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A23DD0-6F33-405E-8925-9755E1234F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1824" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Créer dans l'application des pages avec la même chose que sur le wpf</t>
   </si>
@@ -45,25 +45,34 @@
     <t xml:space="preserve">Ajouter un cœur pour ajouter des ingrédient favoris et si il n'y en a plus les ajouters dans la liste de course. </t>
   </si>
   <si>
-    <t>Ajouter un truc sur l'écran de loggin pour que les utilisateur vois le mot de passe quand ils écrivent</t>
-  </si>
-  <si>
-    <t>Ajouter une page mot de passe perdu</t>
-  </si>
-  <si>
     <t>Ajouter dans l'application se desinscrire pour supprimé le compte et l'adresse email de la base de donné</t>
   </si>
   <si>
-    <t>Changé la page de supabase de confirmation d'inscription</t>
-  </si>
-  <si>
     <t>Pouvoir relié plusieurs compte</t>
   </si>
   <si>
-    <t>Scanné recette de cusine avec téléphone mettre ingrédient et recette au bon endroit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scanné ticket de caisse pour envoyé les ingrédients dans la partie ingrédient et récupéré les prix des ingrédients et le nom du supermarché </t>
+  </si>
+  <si>
+    <t>Trouvé un mode internationale pour traduire mon application en toute les langues .</t>
+  </si>
+  <si>
+    <t>Ajouté Calculatrice sous la liste de course et faire que quand on clique sur la liste de course l'ingrédient part dans ingrédients</t>
+  </si>
+  <si>
+    <t>Mettre un bouton dans le menu aléatoire Si il manque des ingrédients Si ajouter ingrédient dans la liste de course?*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A faire quand y a le temps </t>
+  </si>
+  <si>
+    <t>Demain</t>
+  </si>
+  <si>
+    <t>Changé Couleur de fond quand écran sombre sur téléphone</t>
+  </si>
+  <si>
+    <t>Pouvoir sélectionner plusieurs article de course ou toute la liste de course pour tout supprimé</t>
   </si>
 </sst>
 </file>
@@ -384,78 +393,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B13"/>
+  <dimension ref="B2:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="94.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>11</v>
+    <row r="17" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>